<commit_message>
Commit for marks entry and month end report changes
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/FeeReportsData.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/FeeReportsData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
   <si>
     <t>Academic Year</t>
   </si>
@@ -136,18 +136,37 @@
   </si>
   <si>
     <t>STD 10</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,53 +267,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -763,15 +788,410 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -792,71 +1212,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -866,293 +1226,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1173,21 +1247,103 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1208,123 +1364,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>